<commit_message>
Added calculations and evaluation for corpus 3
</commit_message>
<xml_diff>
--- a/statistics_by_versions.xlsx
+++ b/statistics_by_versions.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MASTER\TMF\Software-Disambiguation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED4D3CD4-B1A4-491E-986A-B6678CA772A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8474A846-1FD3-4D2F-BCD9-A322582F6929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{761929B9-5547-4A46-AB35-1FD98812C8E9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Statistics" sheetId="1" r:id="rId1"/>
+    <sheet name="Evalua" sheetId="3" r:id="rId2"/>
+    <sheet name="Legend" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
   <si>
     <t>Version</t>
   </si>
@@ -63,13 +65,67 @@
   </si>
   <si>
     <t>avg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statistics </t>
+  </si>
+  <si>
+    <t>Version of the corpus</t>
+  </si>
+  <si>
+    <t>calculated similarities of names</t>
+  </si>
+  <si>
+    <t>calculated similarities of authors</t>
+  </si>
+  <si>
+    <t>calculated similarities of keywordss</t>
+  </si>
+  <si>
+    <t>calculated similarities of paragraphs</t>
+  </si>
+  <si>
+    <t>averaged similarities per row</t>
+  </si>
+  <si>
+    <t>minimum similarity per row</t>
+  </si>
+  <si>
+    <t>maximum similarity per row</t>
+  </si>
+  <si>
+    <t>Evaluation</t>
+  </si>
+  <si>
+    <t>MRR@1</t>
+  </si>
+  <si>
+    <t>R-Precision</t>
+  </si>
+  <si>
+    <t>Full MRR</t>
+  </si>
+  <si>
+    <t>the proportion of cases where the correct item appears in the very first position</t>
+  </si>
+  <si>
+    <t>the fraction of all true items that are retrieved within the top R results, where R is the number of true items for that query</t>
+  </si>
+  <si>
+    <t>the average over all queries of 1 divided by the rank of the first correct item</t>
+  </si>
+  <si>
+    <t>3(with negatives)</t>
+  </si>
+  <si>
+    <t>3 (only positives)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +142,15 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="238"/>
@@ -109,14 +174,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -449,15 +517,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B254F3F3-2D58-4C1D-A87C-56C974B5A226}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,17 +541,17 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -502,17 +570,17 @@
       <c r="F2">
         <v>0.40820000000000001</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>0.4456</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>0.11650000000000001</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>0.88970000000000005</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -528,17 +596,17 @@
       <c r="F3">
         <v>-9.7999999999999997E-3</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>0.19650000000000001</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>-4.41E-2</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.56620000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -554,17 +622,17 @@
       <c r="F4">
         <v>0.69679999999999997</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>0.63929999999999998</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>0.52669999999999995</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2</v>
       </c>
@@ -583,17 +651,17 @@
       <c r="F5">
         <v>0.2293</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>0.42730000000000001</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>6.7100000000000007E-2</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>0.88539999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -609,17 +677,17 @@
       <c r="F6">
         <v>-0.1201</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>7.7200000000000005E-2</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>-0.18709999999999999</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>0.3725</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -635,13 +703,193 @@
       <c r="F7">
         <v>0.92090000000000005</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>0.85399999999999998</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>0.65110000000000001</v>
       </c>
-      <c r="I7">
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>0.84989999999999999</v>
+      </c>
+      <c r="D8">
+        <v>0.5292</v>
+      </c>
+      <c r="E8">
+        <v>0.1023</v>
+      </c>
+      <c r="F8">
+        <v>0.29139999999999999</v>
+      </c>
+      <c r="G8">
+        <v>0.61939999999999995</v>
+      </c>
+      <c r="H8">
+        <v>0.47070000000000001</v>
+      </c>
+      <c r="I8">
+        <v>9.1200000000000003E-2</v>
+      </c>
+      <c r="J8">
+        <v>0.89649999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>-0.17</v>
+      </c>
+      <c r="F9">
+        <v>-0.10879999999999999</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0.10059999999999999</v>
+      </c>
+      <c r="I9">
+        <v>-0.17</v>
+      </c>
+      <c r="J9">
+        <v>0.3725</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="F10">
+        <v>0.92090000000000005</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>0.98040000000000005</v>
+      </c>
+      <c r="D11">
+        <v>0.53469999999999995</v>
+      </c>
+      <c r="E11">
+        <v>0.15659999999999999</v>
+      </c>
+      <c r="F11">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="G11">
+        <v>0.94910000000000005</v>
+      </c>
+      <c r="H11">
+        <v>0.57199999999999995</v>
+      </c>
+      <c r="I11">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="J11">
+        <v>0.99280000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>-0.1245</v>
+      </c>
+      <c r="F12">
+        <v>-1.9599999999999999E-2</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0.31209999999999999</v>
+      </c>
+      <c r="I12">
+        <v>-0.1245</v>
+      </c>
+      <c r="J12">
+        <v>0.49909999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0.76670000000000005</v>
+      </c>
+      <c r="F13">
+        <v>0.92090000000000005</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0.83709999999999996</v>
+      </c>
+      <c r="I13">
+        <v>0.65110000000000001</v>
+      </c>
+      <c r="J13">
         <v>1</v>
       </c>
     </row>
@@ -649,4 +897,153 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6425285-6100-4E98-A2FC-D250DCE75505}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{C639DC3B-F845-41B2-AEC2-F51A22041684}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4B5C29-B47A-450B-AA49-EF0EDDC02364}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{9FE4479A-6A4C-4B90-8396-FAAA5CD4A129}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Turned problem into binary classification
</commit_message>
<xml_diff>
--- a/statistics_by_versions.xlsx
+++ b/statistics_by_versions.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MASTER\TMF\Software-Disambiguation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E224DC-1925-4924-A6E4-605C638E05AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380AAE6E-5A64-454F-B1F7-C01B2266F3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="1" xr2:uid="{761929B9-5547-4A46-AB35-1FD98812C8E9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="2" activeTab="2" xr2:uid="{761929B9-5547-4A46-AB35-1FD98812C8E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="1" r:id="rId1"/>
-    <sheet name="Evalua" sheetId="3" r:id="rId2"/>
-    <sheet name="Legend" sheetId="2" r:id="rId3"/>
+    <sheet name="Eval (ranking)" sheetId="3" r:id="rId2"/>
+    <sheet name="Eval (binary)" sheetId="4" r:id="rId3"/>
+    <sheet name="Legend" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="68">
   <si>
     <t>Version</t>
   </si>
@@ -94,9 +95,6 @@
     <t>maximum similarity per row</t>
   </si>
   <si>
-    <t>Evaluation</t>
-  </si>
-  <si>
     <t>MRR@1</t>
   </si>
   <si>
@@ -191,6 +189,60 @@
   </si>
   <si>
     <t>3 (avg)</t>
+  </si>
+  <si>
+    <t>Evaluation (ranked)</t>
+  </si>
+  <si>
+    <t>Evaluation (binary)</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F1 score</t>
+  </si>
+  <si>
+    <t>3(avg)</t>
+  </si>
+  <si>
+    <t>3(min)</t>
+  </si>
+  <si>
+    <t>3(max)</t>
+  </si>
+  <si>
+    <t>1(avg)</t>
+  </si>
+  <si>
+    <t>1(min)</t>
+  </si>
+  <si>
+    <t>1(max)</t>
+  </si>
+  <si>
+    <t>2(avg)</t>
+  </si>
+  <si>
+    <t>2(min)</t>
+  </si>
+  <si>
+    <t>2(max)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1 score </t>
+  </si>
+  <si>
+    <t>proportion of predicted positive cases that are actually positive</t>
+  </si>
+  <si>
+    <t>proportion of actual positive cases that predictions correctly identify</t>
+  </si>
+  <si>
+    <t>harmonic mean of precision and recall, balancing both into a single metric</t>
   </si>
 </sst>
 </file>
@@ -787,7 +839,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -877,7 +929,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -975,7 +1027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6425285-6100-4E98-A2FC-D250DCE75505}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -989,97 +1041,97 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>36</v>
-      </c>
-      <c r="D3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>42</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
         <v>44</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>45</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
         <v>47</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>48</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1092,15 +1144,173 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4B5C29-B47A-450B-AA49-EF0EDDC02364}">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F7A07D-9167-47BA-AC04-19E90D9369D6}">
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.45</v>
+      </c>
+      <c r="D2">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.01</v>
+      </c>
+      <c r="D3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5">
+        <v>0.37</v>
+      </c>
+      <c r="C5">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D5">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6">
+        <v>0.62</v>
+      </c>
+      <c r="C6">
+        <v>0.02</v>
+      </c>
+      <c r="D6">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7">
+        <v>0.1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8">
+        <v>0.44</v>
+      </c>
+      <c r="C8">
+        <v>0.82</v>
+      </c>
+      <c r="D8">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9">
+        <v>0.17</v>
+      </c>
+      <c r="C9">
+        <v>0.01</v>
+      </c>
+      <c r="D9">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10">
+        <v>0.23</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0.38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4B5C29-B47A-450B-AA49-EF0EDDC02364}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
@@ -1172,29 +1382,56 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated model code and results
</commit_message>
<xml_diff>
--- a/statistics_by_versions.xlsx
+++ b/statistics_by_versions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MASTER\TMF\Software-Disambiguation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC1BD32-5679-4B28-80B2-BB3A027515FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F7AF64-3E6C-49B3-8EFA-A57EAA7AE355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" firstSheet="2" activeTab="2" xr2:uid="{761929B9-5547-4A46-AB35-1FD98812C8E9}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="79">
   <si>
     <t>Version</t>
   </si>
@@ -267,6 +267,17 @@
   </si>
   <si>
     <t>3(Neural Net)</t>
+  </si>
+  <si>
+    <t>Univariate (name, keywords, paragraph)</t>
+  </si>
+  <si>
+    <t>Multivariate (all metrics,
+ without missing indicator)</t>
+  </si>
+  <si>
+    <t>With name, keywords, paragraph 
+and their missing indicator</t>
   </si>
 </sst>
 </file>
@@ -326,10 +337,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1169,15 +1183,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F7A07D-9167-47BA-AC04-19E90D9369D6}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1426,7 +1440,7 @@
         <v>75</v>
       </c>
       <c r="B15">
-        <v>0.82</v>
+        <v>0.83</v>
       </c>
       <c r="C15">
         <v>0.89</v>
@@ -1442,6 +1456,366 @@
       </c>
       <c r="G15">
         <v>0.87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C17">
+        <v>0.9</v>
+      </c>
+      <c r="D17">
+        <v>0.7</v>
+      </c>
+      <c r="E17">
+        <v>0.59</v>
+      </c>
+      <c r="F17">
+        <v>0.91</v>
+      </c>
+      <c r="G17">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18">
+        <v>0.79</v>
+      </c>
+      <c r="C18">
+        <v>0.83</v>
+      </c>
+      <c r="D18">
+        <v>0.81</v>
+      </c>
+      <c r="E18">
+        <v>0.8</v>
+      </c>
+      <c r="F18">
+        <v>0.82</v>
+      </c>
+      <c r="G18">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19">
+        <v>0.77</v>
+      </c>
+      <c r="C19">
+        <v>0.91</v>
+      </c>
+      <c r="D19">
+        <v>0.83</v>
+      </c>
+      <c r="E19">
+        <v>0.77</v>
+      </c>
+      <c r="F19">
+        <v>0.89</v>
+      </c>
+      <c r="G19">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20">
+        <v>0.77</v>
+      </c>
+      <c r="C20">
+        <v>0.93</v>
+      </c>
+      <c r="D20">
+        <v>0.84</v>
+      </c>
+      <c r="E20">
+        <v>0.76</v>
+      </c>
+      <c r="F20">
+        <v>0.94</v>
+      </c>
+      <c r="G20">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21">
+        <v>0.79</v>
+      </c>
+      <c r="C21">
+        <v>0.84</v>
+      </c>
+      <c r="D21">
+        <v>0.81</v>
+      </c>
+      <c r="E21">
+        <v>0.76</v>
+      </c>
+      <c r="F21">
+        <v>0.88</v>
+      </c>
+      <c r="G21">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23">
+        <v>0.6</v>
+      </c>
+      <c r="C23">
+        <v>0.9</v>
+      </c>
+      <c r="D23">
+        <v>0.72</v>
+      </c>
+      <c r="E23">
+        <v>0.6</v>
+      </c>
+      <c r="F23">
+        <v>0.93</v>
+      </c>
+      <c r="G23">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24">
+        <v>0.84</v>
+      </c>
+      <c r="C24">
+        <v>0.86</v>
+      </c>
+      <c r="D24">
+        <v>0.85</v>
+      </c>
+      <c r="E24">
+        <v>0.85</v>
+      </c>
+      <c r="F24">
+        <v>0.89</v>
+      </c>
+      <c r="G24">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25">
+        <v>0.84</v>
+      </c>
+      <c r="C25">
+        <v>0.9</v>
+      </c>
+      <c r="D25">
+        <v>0.87</v>
+      </c>
+      <c r="E25">
+        <v>0.85</v>
+      </c>
+      <c r="F25">
+        <v>0.91</v>
+      </c>
+      <c r="G25">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26">
+        <v>0.84</v>
+      </c>
+      <c r="C26">
+        <v>0.92</v>
+      </c>
+      <c r="D26">
+        <v>0.88</v>
+      </c>
+      <c r="E26">
+        <v>0.83</v>
+      </c>
+      <c r="F26">
+        <v>0.95</v>
+      </c>
+      <c r="G26">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27">
+        <v>0.82</v>
+      </c>
+      <c r="C27">
+        <v>0.86</v>
+      </c>
+      <c r="D27">
+        <v>0.84</v>
+      </c>
+      <c r="E27">
+        <v>0.78</v>
+      </c>
+      <c r="F27">
+        <v>0.84</v>
+      </c>
+      <c r="G27">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29">
+        <v>0.6</v>
+      </c>
+      <c r="C29">
+        <v>0.91</v>
+      </c>
+      <c r="D29">
+        <v>0.73</v>
+      </c>
+      <c r="E29">
+        <v>0.61</v>
+      </c>
+      <c r="F29">
+        <v>0.92</v>
+      </c>
+      <c r="G29">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30">
+        <v>0.79</v>
+      </c>
+      <c r="C30">
+        <v>0.83</v>
+      </c>
+      <c r="D30">
+        <v>0.81</v>
+      </c>
+      <c r="E30">
+        <v>0.8</v>
+      </c>
+      <c r="F30">
+        <v>0.82</v>
+      </c>
+      <c r="G30">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31">
+        <v>0.77</v>
+      </c>
+      <c r="C31">
+        <v>0.91</v>
+      </c>
+      <c r="D31">
+        <v>0.83</v>
+      </c>
+      <c r="E31">
+        <v>0.77</v>
+      </c>
+      <c r="F31">
+        <v>0.89</v>
+      </c>
+      <c r="G31">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>74</v>
+      </c>
+      <c r="B32">
+        <v>0.77</v>
+      </c>
+      <c r="C32">
+        <v>0.93</v>
+      </c>
+      <c r="D32">
+        <v>0.84</v>
+      </c>
+      <c r="E32">
+        <v>0.76</v>
+      </c>
+      <c r="F32">
+        <v>0.94</v>
+      </c>
+      <c r="G32">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33">
+        <v>0.79</v>
+      </c>
+      <c r="C33">
+        <v>0.88</v>
+      </c>
+      <c r="D33">
+        <v>0.83</v>
+      </c>
+      <c r="E33">
+        <v>0.77</v>
+      </c>
+      <c r="F33">
+        <v>0.89</v>
+      </c>
+      <c r="G33">
+        <v>0.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Versions 3.8, 3.9, 3.10, 3.11 and 3.12
</commit_message>
<xml_diff>
--- a/statistics_by_versions.xlsx
+++ b/statistics_by_versions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MASTER\TMF\Software-Disambiguation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5009B9-BF18-416C-A621-A47BF43ADE0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDECD07-2A2A-4A94-8974-0707889B1D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{761929B9-5547-4A46-AB35-1FD98812C8E9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="2" xr2:uid="{761929B9-5547-4A46-AB35-1FD98812C8E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="143">
   <si>
     <t>Version</t>
   </si>
@@ -413,6 +413,66 @@
   </si>
   <si>
     <t>3.8(Neural Net)</t>
+  </si>
+  <si>
+    <t>3.9(Logistic regression)</t>
+  </si>
+  <si>
+    <t>3.9(Random Forest)</t>
+  </si>
+  <si>
+    <t>3.9(XGBoost)</t>
+  </si>
+  <si>
+    <t>3.9(LightGBM)</t>
+  </si>
+  <si>
+    <t>3.9(Neural Net)</t>
+  </si>
+  <si>
+    <t>3.10(Logistic regression)</t>
+  </si>
+  <si>
+    <t>3.10(Random Forest)</t>
+  </si>
+  <si>
+    <t>3.10(XGBoost)</t>
+  </si>
+  <si>
+    <t>3.10(LightGBM)</t>
+  </si>
+  <si>
+    <t>3.10(Neural Net)</t>
+  </si>
+  <si>
+    <t>3.11(Logistic regression)</t>
+  </si>
+  <si>
+    <t>3.11(Random Forest)</t>
+  </si>
+  <si>
+    <t>3.11(XGBoost)</t>
+  </si>
+  <si>
+    <t>3.11(LightGBM)</t>
+  </si>
+  <si>
+    <t>3.11(Neural Net)</t>
+  </si>
+  <si>
+    <t>3.12(Logistic regression)</t>
+  </si>
+  <si>
+    <t>3.12(Random Forest)</t>
+  </si>
+  <si>
+    <t>3.12(XGBoost)</t>
+  </si>
+  <si>
+    <t>3.12(LightGBM)</t>
+  </si>
+  <si>
+    <t>3.12(Neural Net)</t>
   </si>
 </sst>
 </file>
@@ -1318,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F7A07D-9167-47BA-AC04-19E90D9369D6}">
-  <dimension ref="A1:G196"/>
+  <dimension ref="A1:G268"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="Q156" sqref="Q156"/>
+    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
+      <selection activeCell="K267" sqref="K267"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5198,6 +5258,1446 @@
         <v>0.84</v>
       </c>
     </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A197" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A198" t="s">
+        <v>123</v>
+      </c>
+      <c r="B198">
+        <v>0.64</v>
+      </c>
+      <c r="C198">
+        <v>0.92</v>
+      </c>
+      <c r="D198">
+        <v>0.75</v>
+      </c>
+      <c r="E198">
+        <v>0.65</v>
+      </c>
+      <c r="F198">
+        <v>0.93</v>
+      </c>
+      <c r="G198">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A199" t="s">
+        <v>124</v>
+      </c>
+      <c r="B199">
+        <v>0.87</v>
+      </c>
+      <c r="C199">
+        <v>0.9</v>
+      </c>
+      <c r="D199">
+        <v>0.89</v>
+      </c>
+      <c r="E199">
+        <v>0.86</v>
+      </c>
+      <c r="F199">
+        <v>0.91</v>
+      </c>
+      <c r="G199">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A200" t="s">
+        <v>125</v>
+      </c>
+      <c r="B200">
+        <v>0.87</v>
+      </c>
+      <c r="C200">
+        <v>0.93</v>
+      </c>
+      <c r="D200">
+        <v>0.9</v>
+      </c>
+      <c r="E200">
+        <v>0.86</v>
+      </c>
+      <c r="F200">
+        <v>0.96</v>
+      </c>
+      <c r="G200">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A201" t="s">
+        <v>126</v>
+      </c>
+      <c r="B201">
+        <v>0.87</v>
+      </c>
+      <c r="C201">
+        <v>0.94</v>
+      </c>
+      <c r="D201">
+        <v>0.9</v>
+      </c>
+      <c r="E201">
+        <v>0.86</v>
+      </c>
+      <c r="F201">
+        <v>0.97</v>
+      </c>
+      <c r="G201">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A202" t="s">
+        <v>127</v>
+      </c>
+      <c r="B202">
+        <v>0.85</v>
+      </c>
+      <c r="C202">
+        <v>0.88</v>
+      </c>
+      <c r="D202">
+        <v>0.87</v>
+      </c>
+      <c r="E202">
+        <v>0.81</v>
+      </c>
+      <c r="F202">
+        <v>0.92</v>
+      </c>
+      <c r="G202">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A203" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A204" t="s">
+        <v>123</v>
+      </c>
+      <c r="B204">
+        <v>0.59</v>
+      </c>
+      <c r="C204">
+        <v>0.9</v>
+      </c>
+      <c r="D204">
+        <v>0.72</v>
+      </c>
+      <c r="E204">
+        <v>0.6</v>
+      </c>
+      <c r="F204">
+        <v>0.92</v>
+      </c>
+      <c r="G204">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A205" t="s">
+        <v>124</v>
+      </c>
+      <c r="B205">
+        <v>0.86</v>
+      </c>
+      <c r="C205">
+        <v>0.9</v>
+      </c>
+      <c r="D205">
+        <v>0.88</v>
+      </c>
+      <c r="E205">
+        <v>0.86</v>
+      </c>
+      <c r="F205">
+        <v>0.92</v>
+      </c>
+      <c r="G205">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A206" t="s">
+        <v>125</v>
+      </c>
+      <c r="B206">
+        <v>0.87</v>
+      </c>
+      <c r="C206">
+        <v>0.93</v>
+      </c>
+      <c r="D206">
+        <v>0.9</v>
+      </c>
+      <c r="E206">
+        <v>0.86</v>
+      </c>
+      <c r="F206">
+        <v>0.96</v>
+      </c>
+      <c r="G206">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
+        <v>126</v>
+      </c>
+      <c r="B207">
+        <v>0.87</v>
+      </c>
+      <c r="C207">
+        <v>0.94</v>
+      </c>
+      <c r="D207">
+        <v>0.9</v>
+      </c>
+      <c r="E207">
+        <v>0.86</v>
+      </c>
+      <c r="F207">
+        <v>0.97</v>
+      </c>
+      <c r="G207">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A208" t="s">
+        <v>127</v>
+      </c>
+      <c r="B208">
+        <v>0.83</v>
+      </c>
+      <c r="C208">
+        <v>0.86</v>
+      </c>
+      <c r="D208">
+        <v>0.85</v>
+      </c>
+      <c r="E208">
+        <v>0.8</v>
+      </c>
+      <c r="F208">
+        <v>0.86</v>
+      </c>
+      <c r="G208">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A209" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>123</v>
+      </c>
+      <c r="B210">
+        <v>0.61</v>
+      </c>
+      <c r="C210">
+        <v>0.9</v>
+      </c>
+      <c r="D210">
+        <v>0.73</v>
+      </c>
+      <c r="E210">
+        <v>0.62</v>
+      </c>
+      <c r="F210">
+        <v>0.93</v>
+      </c>
+      <c r="G210">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>124</v>
+      </c>
+      <c r="B211">
+        <v>0.88</v>
+      </c>
+      <c r="C211">
+        <v>0.9</v>
+      </c>
+      <c r="D211">
+        <v>0.89</v>
+      </c>
+      <c r="E211">
+        <v>0.86</v>
+      </c>
+      <c r="F211">
+        <v>0.91</v>
+      </c>
+      <c r="G211">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>125</v>
+      </c>
+      <c r="B212">
+        <v>0.87</v>
+      </c>
+      <c r="C212">
+        <v>0.94</v>
+      </c>
+      <c r="D212">
+        <v>0.9</v>
+      </c>
+      <c r="E212">
+        <v>0.85</v>
+      </c>
+      <c r="F212">
+        <v>0.95</v>
+      </c>
+      <c r="G212">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>126</v>
+      </c>
+      <c r="B213">
+        <v>0.86</v>
+      </c>
+      <c r="C213">
+        <v>0.94</v>
+      </c>
+      <c r="D213">
+        <v>0.9</v>
+      </c>
+      <c r="E213">
+        <v>0.83</v>
+      </c>
+      <c r="F213">
+        <v>0.96</v>
+      </c>
+      <c r="G213">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>127</v>
+      </c>
+      <c r="B214">
+        <v>0.85</v>
+      </c>
+      <c r="C214">
+        <v>0.87</v>
+      </c>
+      <c r="D214">
+        <v>0.86</v>
+      </c>
+      <c r="E214">
+        <v>0.83</v>
+      </c>
+      <c r="F214">
+        <v>0.88</v>
+      </c>
+      <c r="G214">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>128</v>
+      </c>
+      <c r="B216">
+        <v>0.72</v>
+      </c>
+      <c r="C216">
+        <v>0.93</v>
+      </c>
+      <c r="D216">
+        <v>0.91</v>
+      </c>
+      <c r="E216">
+        <v>0.71</v>
+      </c>
+      <c r="F216">
+        <v>0.94</v>
+      </c>
+      <c r="G216">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>129</v>
+      </c>
+      <c r="B217">
+        <v>0.88</v>
+      </c>
+      <c r="C217">
+        <v>0.9</v>
+      </c>
+      <c r="D217">
+        <v>0.89</v>
+      </c>
+      <c r="E217">
+        <v>0.86</v>
+      </c>
+      <c r="F217">
+        <v>0.92</v>
+      </c>
+      <c r="G217">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>130</v>
+      </c>
+      <c r="B218">
+        <v>0.87</v>
+      </c>
+      <c r="C218">
+        <v>0.93</v>
+      </c>
+      <c r="D218">
+        <v>0.9</v>
+      </c>
+      <c r="E218">
+        <v>0.87</v>
+      </c>
+      <c r="F218">
+        <v>0.95</v>
+      </c>
+      <c r="G218">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>131</v>
+      </c>
+      <c r="B219">
+        <v>0.87</v>
+      </c>
+      <c r="C219">
+        <v>0.94</v>
+      </c>
+      <c r="D219">
+        <v>0.9</v>
+      </c>
+      <c r="E219">
+        <v>0.85</v>
+      </c>
+      <c r="F219">
+        <v>0.96</v>
+      </c>
+      <c r="G219">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>132</v>
+      </c>
+      <c r="B220">
+        <v>0.85</v>
+      </c>
+      <c r="C220">
+        <v>0.88</v>
+      </c>
+      <c r="D220">
+        <v>0.87</v>
+      </c>
+      <c r="E220">
+        <v>0.82</v>
+      </c>
+      <c r="F220">
+        <v>0.92</v>
+      </c>
+      <c r="G220">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A221" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>128</v>
+      </c>
+      <c r="B222">
+        <v>0.67</v>
+      </c>
+      <c r="C222">
+        <v>0.92</v>
+      </c>
+      <c r="D222">
+        <v>0.77</v>
+      </c>
+      <c r="E222">
+        <v>0.67</v>
+      </c>
+      <c r="F222">
+        <v>0.93</v>
+      </c>
+      <c r="G222">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>129</v>
+      </c>
+      <c r="B223">
+        <v>0.86</v>
+      </c>
+      <c r="C223">
+        <v>0.9</v>
+      </c>
+      <c r="D223">
+        <v>0.88</v>
+      </c>
+      <c r="E223">
+        <v>0.85</v>
+      </c>
+      <c r="F223">
+        <v>0.92</v>
+      </c>
+      <c r="G223">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>130</v>
+      </c>
+      <c r="B224">
+        <v>0.88</v>
+      </c>
+      <c r="C224">
+        <v>0.93</v>
+      </c>
+      <c r="D224">
+        <v>0.9</v>
+      </c>
+      <c r="E224">
+        <v>0.87</v>
+      </c>
+      <c r="F224">
+        <v>0.95</v>
+      </c>
+      <c r="G224">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>131</v>
+      </c>
+      <c r="B225">
+        <v>0.87</v>
+      </c>
+      <c r="C225">
+        <v>0.94</v>
+      </c>
+      <c r="D225">
+        <v>0.9</v>
+      </c>
+      <c r="E225">
+        <v>0.85</v>
+      </c>
+      <c r="F225">
+        <v>0.96</v>
+      </c>
+      <c r="G225">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>132</v>
+      </c>
+      <c r="B226">
+        <v>0.82</v>
+      </c>
+      <c r="C226">
+        <v>0.86</v>
+      </c>
+      <c r="D226">
+        <v>0.84</v>
+      </c>
+      <c r="E226">
+        <v>0.81</v>
+      </c>
+      <c r="F226">
+        <v>0.85</v>
+      </c>
+      <c r="G226">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A227" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>128</v>
+      </c>
+      <c r="B228">
+        <v>0.69</v>
+      </c>
+      <c r="C228">
+        <v>0.92</v>
+      </c>
+      <c r="D228">
+        <v>0.79</v>
+      </c>
+      <c r="E228">
+        <v>0.69</v>
+      </c>
+      <c r="F228">
+        <v>0.92</v>
+      </c>
+      <c r="G228">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>129</v>
+      </c>
+      <c r="B229">
+        <v>0.87</v>
+      </c>
+      <c r="C229">
+        <v>0.89</v>
+      </c>
+      <c r="D229">
+        <v>0.88</v>
+      </c>
+      <c r="E229">
+        <v>0.86</v>
+      </c>
+      <c r="F229">
+        <v>0.91</v>
+      </c>
+      <c r="G229">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>130</v>
+      </c>
+      <c r="B230">
+        <v>0.87</v>
+      </c>
+      <c r="C230">
+        <v>0.93</v>
+      </c>
+      <c r="D230">
+        <v>0.9</v>
+      </c>
+      <c r="E230">
+        <v>0.86</v>
+      </c>
+      <c r="F230">
+        <v>0.94</v>
+      </c>
+      <c r="G230">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>131</v>
+      </c>
+      <c r="B231">
+        <v>0.86</v>
+      </c>
+      <c r="C231">
+        <v>0.94</v>
+      </c>
+      <c r="D231">
+        <v>0.9</v>
+      </c>
+      <c r="E231">
+        <v>0.84</v>
+      </c>
+      <c r="F231">
+        <v>0.96</v>
+      </c>
+      <c r="G231">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>132</v>
+      </c>
+      <c r="B232">
+        <v>0.86</v>
+      </c>
+      <c r="C232">
+        <v>0.86</v>
+      </c>
+      <c r="D232">
+        <v>0.86</v>
+      </c>
+      <c r="E232">
+        <v>0.82</v>
+      </c>
+      <c r="F232">
+        <v>0.87</v>
+      </c>
+      <c r="G232">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A234" t="s">
+        <v>133</v>
+      </c>
+      <c r="B234">
+        <v>0.7</v>
+      </c>
+      <c r="C234">
+        <v>0.93</v>
+      </c>
+      <c r="D234">
+        <v>0.8</v>
+      </c>
+      <c r="E234">
+        <v>0.7</v>
+      </c>
+      <c r="F234">
+        <v>0.94</v>
+      </c>
+      <c r="G234">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A235" t="s">
+        <v>134</v>
+      </c>
+      <c r="B235">
+        <v>0.88</v>
+      </c>
+      <c r="C235">
+        <v>0.89</v>
+      </c>
+      <c r="D235">
+        <v>0.88</v>
+      </c>
+      <c r="E235">
+        <v>0.85</v>
+      </c>
+      <c r="F235">
+        <v>0.92</v>
+      </c>
+      <c r="G235">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A236" t="s">
+        <v>135</v>
+      </c>
+      <c r="B236">
+        <v>0.88</v>
+      </c>
+      <c r="C236">
+        <v>0.93</v>
+      </c>
+      <c r="D236">
+        <v>0.9</v>
+      </c>
+      <c r="E236">
+        <v>0.87</v>
+      </c>
+      <c r="F236">
+        <v>0.95</v>
+      </c>
+      <c r="G236">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A237" t="s">
+        <v>136</v>
+      </c>
+      <c r="B237">
+        <v>0.86</v>
+      </c>
+      <c r="C237">
+        <v>0.94</v>
+      </c>
+      <c r="D237">
+        <v>0.9</v>
+      </c>
+      <c r="E237">
+        <v>0.85</v>
+      </c>
+      <c r="F237">
+        <v>0.95</v>
+      </c>
+      <c r="G237">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A238" t="s">
+        <v>137</v>
+      </c>
+      <c r="B238">
+        <v>0.85</v>
+      </c>
+      <c r="C238">
+        <v>0.86</v>
+      </c>
+      <c r="D238">
+        <v>0.86</v>
+      </c>
+      <c r="E238">
+        <v>0.81</v>
+      </c>
+      <c r="F238">
+        <v>0.92</v>
+      </c>
+      <c r="G238">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A239" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A240" t="s">
+        <v>133</v>
+      </c>
+      <c r="B240">
+        <v>0.67</v>
+      </c>
+      <c r="C240">
+        <v>0.92</v>
+      </c>
+      <c r="D240">
+        <v>0.77</v>
+      </c>
+      <c r="E240">
+        <v>0.66</v>
+      </c>
+      <c r="F240">
+        <v>0.92</v>
+      </c>
+      <c r="G240">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A241" t="s">
+        <v>134</v>
+      </c>
+      <c r="B241">
+        <v>0.86</v>
+      </c>
+      <c r="C241">
+        <v>0.88</v>
+      </c>
+      <c r="D241">
+        <v>0.87</v>
+      </c>
+      <c r="E241">
+        <v>0.85</v>
+      </c>
+      <c r="F241">
+        <v>0.92</v>
+      </c>
+      <c r="G241">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A242" t="s">
+        <v>135</v>
+      </c>
+      <c r="B242">
+        <v>0.87</v>
+      </c>
+      <c r="C242">
+        <v>0.93</v>
+      </c>
+      <c r="D242">
+        <v>0.9</v>
+      </c>
+      <c r="E242">
+        <v>0.86</v>
+      </c>
+      <c r="F242">
+        <v>0.94</v>
+      </c>
+      <c r="G242">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A243" t="s">
+        <v>136</v>
+      </c>
+      <c r="B243">
+        <v>0.86</v>
+      </c>
+      <c r="C243">
+        <v>0.94</v>
+      </c>
+      <c r="D243">
+        <v>0.9</v>
+      </c>
+      <c r="E243">
+        <v>0.85</v>
+      </c>
+      <c r="F243">
+        <v>0.95</v>
+      </c>
+      <c r="G243">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A244" t="s">
+        <v>137</v>
+      </c>
+      <c r="B244">
+        <v>0.82</v>
+      </c>
+      <c r="C244">
+        <v>0.84</v>
+      </c>
+      <c r="D244">
+        <v>0.83</v>
+      </c>
+      <c r="E244">
+        <v>0.79</v>
+      </c>
+      <c r="F244">
+        <v>0.84</v>
+      </c>
+      <c r="G244">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A245" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A246" t="s">
+        <v>133</v>
+      </c>
+      <c r="B246">
+        <v>0.68</v>
+      </c>
+      <c r="C246">
+        <v>0.92</v>
+      </c>
+      <c r="D246">
+        <v>0.78</v>
+      </c>
+      <c r="E246">
+        <v>0.69</v>
+      </c>
+      <c r="F246">
+        <v>0.93</v>
+      </c>
+      <c r="G246">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A247" t="s">
+        <v>134</v>
+      </c>
+      <c r="B247">
+        <v>0.88</v>
+      </c>
+      <c r="C247">
+        <v>0.88</v>
+      </c>
+      <c r="D247">
+        <v>0.88</v>
+      </c>
+      <c r="E247">
+        <v>0.85</v>
+      </c>
+      <c r="F247">
+        <v>0.9</v>
+      </c>
+      <c r="G247">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A248" t="s">
+        <v>135</v>
+      </c>
+      <c r="B248">
+        <v>0.86</v>
+      </c>
+      <c r="C248">
+        <v>0.92</v>
+      </c>
+      <c r="D248">
+        <v>0.89</v>
+      </c>
+      <c r="E248">
+        <v>0.86</v>
+      </c>
+      <c r="F248">
+        <v>0.93</v>
+      </c>
+      <c r="G248">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A249" t="s">
+        <v>136</v>
+      </c>
+      <c r="B249">
+        <v>0.85</v>
+      </c>
+      <c r="C249">
+        <v>0.94</v>
+      </c>
+      <c r="D249">
+        <v>0.89</v>
+      </c>
+      <c r="E249">
+        <v>0.84</v>
+      </c>
+      <c r="F249">
+        <v>0.95</v>
+      </c>
+      <c r="G249">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A250" t="s">
+        <v>137</v>
+      </c>
+      <c r="B250">
+        <v>0.86</v>
+      </c>
+      <c r="C250">
+        <v>0.86</v>
+      </c>
+      <c r="D250">
+        <v>0.86</v>
+      </c>
+      <c r="E250">
+        <v>0.81</v>
+      </c>
+      <c r="F250">
+        <v>0.88</v>
+      </c>
+      <c r="G250">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A251" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
+        <v>138</v>
+      </c>
+      <c r="B252">
+        <v>0.64</v>
+      </c>
+      <c r="C252">
+        <v>0.92</v>
+      </c>
+      <c r="D252">
+        <v>0.75</v>
+      </c>
+      <c r="E252">
+        <v>0.65</v>
+      </c>
+      <c r="F252">
+        <v>0.94</v>
+      </c>
+      <c r="G252">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A253" t="s">
+        <v>139</v>
+      </c>
+      <c r="B253">
+        <v>0.89</v>
+      </c>
+      <c r="C253">
+        <v>0.89</v>
+      </c>
+      <c r="D253">
+        <v>0.89</v>
+      </c>
+      <c r="E253">
+        <v>0.88</v>
+      </c>
+      <c r="F253">
+        <v>0.92</v>
+      </c>
+      <c r="G253">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A254" t="s">
+        <v>140</v>
+      </c>
+      <c r="B254">
+        <v>0.88</v>
+      </c>
+      <c r="C254">
+        <v>0.94</v>
+      </c>
+      <c r="D254">
+        <v>0.91</v>
+      </c>
+      <c r="E254">
+        <v>0.88</v>
+      </c>
+      <c r="F254">
+        <v>0.95</v>
+      </c>
+      <c r="G254">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
+        <v>141</v>
+      </c>
+      <c r="B255">
+        <v>0.88</v>
+      </c>
+      <c r="C255">
+        <v>0.94</v>
+      </c>
+      <c r="D255">
+        <v>0.91</v>
+      </c>
+      <c r="E255">
+        <v>0.87</v>
+      </c>
+      <c r="F255">
+        <v>0.94</v>
+      </c>
+      <c r="G255">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A256" t="s">
+        <v>142</v>
+      </c>
+      <c r="B256">
+        <v>0.85</v>
+      </c>
+      <c r="C256">
+        <v>0.86</v>
+      </c>
+      <c r="D256">
+        <v>0.85</v>
+      </c>
+      <c r="E256">
+        <v>0.81</v>
+      </c>
+      <c r="F256">
+        <v>0.94</v>
+      </c>
+      <c r="G256">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="257" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A257" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
+        <v>138</v>
+      </c>
+      <c r="B258">
+        <v>0.59</v>
+      </c>
+      <c r="C258">
+        <v>0.9</v>
+      </c>
+      <c r="D258">
+        <v>0.72</v>
+      </c>
+      <c r="E258">
+        <v>0.6</v>
+      </c>
+      <c r="F258">
+        <v>0.92</v>
+      </c>
+      <c r="G258">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
+        <v>139</v>
+      </c>
+      <c r="B259">
+        <v>0.88</v>
+      </c>
+      <c r="C259">
+        <v>0.89</v>
+      </c>
+      <c r="D259">
+        <v>0.89</v>
+      </c>
+      <c r="E259">
+        <v>0.89</v>
+      </c>
+      <c r="F259">
+        <v>0.91</v>
+      </c>
+      <c r="G259">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A260" t="s">
+        <v>140</v>
+      </c>
+      <c r="B260">
+        <v>0.88</v>
+      </c>
+      <c r="C260">
+        <v>0.93</v>
+      </c>
+      <c r="D260">
+        <v>0.9</v>
+      </c>
+      <c r="E260">
+        <v>0.89</v>
+      </c>
+      <c r="F260">
+        <v>0.94</v>
+      </c>
+      <c r="G260">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A261" t="s">
+        <v>141</v>
+      </c>
+      <c r="B261">
+        <v>0.88</v>
+      </c>
+      <c r="C261">
+        <v>0.94</v>
+      </c>
+      <c r="D261">
+        <v>0.91</v>
+      </c>
+      <c r="E261">
+        <v>0.87</v>
+      </c>
+      <c r="F261">
+        <v>0.94</v>
+      </c>
+      <c r="G261">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A262" t="s">
+        <v>142</v>
+      </c>
+      <c r="B262">
+        <v>0.8</v>
+      </c>
+      <c r="C262">
+        <v>0.88</v>
+      </c>
+      <c r="D262">
+        <v>0.84</v>
+      </c>
+      <c r="E262">
+        <v>0.82</v>
+      </c>
+      <c r="F262">
+        <v>0.86</v>
+      </c>
+      <c r="G262">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="263" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A263" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
+        <v>138</v>
+      </c>
+      <c r="B264">
+        <v>0.61</v>
+      </c>
+      <c r="C264">
+        <v>0.91</v>
+      </c>
+      <c r="D264">
+        <v>0.73</v>
+      </c>
+      <c r="E264">
+        <v>0.62</v>
+      </c>
+      <c r="F264">
+        <v>0.92</v>
+      </c>
+      <c r="G264">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
+        <v>139</v>
+      </c>
+      <c r="B265">
+        <v>0.89</v>
+      </c>
+      <c r="C265">
+        <v>0.89</v>
+      </c>
+      <c r="D265">
+        <v>0.89</v>
+      </c>
+      <c r="E265">
+        <v>0.88</v>
+      </c>
+      <c r="F265">
+        <v>0.92</v>
+      </c>
+      <c r="G265">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
+        <v>140</v>
+      </c>
+      <c r="B266">
+        <v>0.87</v>
+      </c>
+      <c r="C266">
+        <v>0.93</v>
+      </c>
+      <c r="D266">
+        <v>0.9</v>
+      </c>
+      <c r="E266">
+        <v>0.87</v>
+      </c>
+      <c r="F266">
+        <v>0.93</v>
+      </c>
+      <c r="G266">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
+        <v>141</v>
+      </c>
+      <c r="B267">
+        <v>0.86</v>
+      </c>
+      <c r="C267">
+        <v>0.94</v>
+      </c>
+      <c r="D267">
+        <v>0.9</v>
+      </c>
+      <c r="E267">
+        <v>0.86</v>
+      </c>
+      <c r="F267">
+        <v>0.94</v>
+      </c>
+      <c r="G267">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
+        <v>142</v>
+      </c>
+      <c r="B268">
+        <v>0.83</v>
+      </c>
+      <c r="C268">
+        <v>0.85</v>
+      </c>
+      <c r="D268">
+        <v>0.84</v>
+      </c>
+      <c r="E268">
+        <v>0.83</v>
+      </c>
+      <c r="F268">
+        <v>0.87</v>
+      </c>
+      <c r="G268">
+        <v>0.85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5208,7 +6708,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updating the best nodel
</commit_message>
<xml_diff>
--- a/statistics_by_versions.xlsx
+++ b/statistics_by_versions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MASTER\TMF\Software-Disambiguation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BEF0226-523E-441D-AC49-677DFAC00726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC24F4C-DD0E-4039-ABB9-5F61C7FC32D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{761929B9-5547-4A46-AB35-1FD98812C8E9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{761929B9-5547-4A46-AB35-1FD98812C8E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Eval (binary)" sheetId="4" r:id="rId1"/>
@@ -724,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1F7A07D-9167-47BA-AC04-19E90D9369D6}">
   <dimension ref="A1:G253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
-      <selection activeCell="K193" sqref="K193"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4278,10 +4278,10 @@
         <v>0.89</v>
       </c>
       <c r="E178">
-        <v>0.9</v>
+        <v>0.89</v>
       </c>
       <c r="F178">
-        <v>0.93</v>
+        <v>0.92</v>
       </c>
       <c r="G178">
         <v>0.91</v>

</xml_diff>

<commit_message>
Updated versions 3.13, 3.14 and 3.15
</commit_message>
<xml_diff>
--- a/statistics_by_versions.xlsx
+++ b/statistics_by_versions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MASTER\TMF\Software-Disambiguation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFFF530-5E04-43BF-B63D-60328D175636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAAACF5F-F3A9-4B4E-B7CD-DEAB2530995B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{761929B9-5547-4A46-AB35-1FD98812C8E9}"/>
   </bookViews>
@@ -752,7 +752,7 @@
   <dimension ref="A1:G265"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
-      <selection activeCell="E262" sqref="E262"/>
+      <selection activeCell="G266" sqref="G266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5833,22 +5833,22 @@
         <v>100</v>
       </c>
       <c r="B255">
-        <v>0.9</v>
+        <v>0.88</v>
       </c>
       <c r="C255">
         <v>0.89</v>
       </c>
       <c r="D255">
-        <v>0.9</v>
+        <v>0.88</v>
       </c>
       <c r="E255">
         <v>0.89</v>
       </c>
       <c r="F255">
-        <v>0.92</v>
+        <v>0.88</v>
       </c>
       <c r="G255">
-        <v>0.91</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.3">
@@ -5856,22 +5856,22 @@
         <v>101</v>
       </c>
       <c r="B256">
-        <v>0.89</v>
+        <v>0.86</v>
       </c>
       <c r="C256">
         <v>0.92</v>
       </c>
       <c r="D256">
-        <v>0.9</v>
+        <v>0.89</v>
       </c>
       <c r="E256">
-        <v>0.86</v>
+        <v>0.88</v>
       </c>
       <c r="F256">
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
       <c r="G256">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.3">
@@ -5879,19 +5879,19 @@
         <v>102</v>
       </c>
       <c r="B257">
-        <v>0.88</v>
+        <v>0.86</v>
       </c>
       <c r="C257">
-        <v>0.94</v>
+        <v>0.93</v>
       </c>
       <c r="D257">
-        <v>0.91</v>
+        <v>0.89</v>
       </c>
       <c r="E257">
         <v>0.86</v>
       </c>
       <c r="F257">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="G257">
         <v>0.91</v>
@@ -5907,22 +5907,22 @@
         <v>103</v>
       </c>
       <c r="B259">
-        <v>0.9</v>
+        <v>0.89</v>
       </c>
       <c r="C259">
-        <v>0.9</v>
+        <v>0.89</v>
       </c>
       <c r="D259">
-        <v>0.9</v>
+        <v>0.89</v>
       </c>
       <c r="E259">
-        <v>0.88</v>
+        <v>0.9</v>
       </c>
       <c r="F259">
-        <v>0.89</v>
+        <v>0.92</v>
       </c>
       <c r="G259">
-        <v>0.88</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.3">
@@ -5930,22 +5930,22 @@
         <v>104</v>
       </c>
       <c r="B260">
-        <v>0.88</v>
+        <v>0.87</v>
       </c>
       <c r="C260">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="D260">
         <v>0.9</v>
       </c>
       <c r="E260">
-        <v>0.86</v>
+        <v>0.88</v>
       </c>
       <c r="F260">
         <v>0.93</v>
       </c>
       <c r="G260">
-        <v>0.89</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.3">
@@ -5956,19 +5956,19 @@
         <v>0.87</v>
       </c>
       <c r="C261">
-        <v>0.94</v>
+        <v>0.95</v>
       </c>
       <c r="D261">
         <v>0.91</v>
       </c>
       <c r="E261">
-        <v>0.86</v>
+        <v>0.88</v>
       </c>
       <c r="F261">
-        <v>0.94</v>
+        <v>0.95</v>
       </c>
       <c r="G261">
-        <v>0.9</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.3">
@@ -5981,19 +5981,19 @@
         <v>106</v>
       </c>
       <c r="B263">
-        <v>0.89</v>
+        <v>0.88</v>
       </c>
       <c r="C263">
         <v>0.89</v>
       </c>
       <c r="D263">
-        <v>0.89</v>
+        <v>0.88</v>
       </c>
       <c r="E263">
-        <v>0.88</v>
+        <v>0.89</v>
       </c>
       <c r="F263">
-        <v>0.89</v>
+        <v>0.9</v>
       </c>
       <c r="G263">
         <v>0.89</v>
@@ -6013,10 +6013,10 @@
         <v>0.89</v>
       </c>
       <c r="E264">
-        <v>0.88</v>
+        <v>0.87</v>
       </c>
       <c r="F264">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="G264">
         <v>0.9</v>
@@ -6027,16 +6027,16 @@
         <v>108</v>
       </c>
       <c r="B265">
-        <v>0.87</v>
+        <v>0.86</v>
       </c>
       <c r="C265">
         <v>0.93</v>
       </c>
       <c r="D265">
-        <v>0.9</v>
+        <v>0.89</v>
       </c>
       <c r="E265">
-        <v>0.87</v>
+        <v>0.85</v>
       </c>
       <c r="F265">
         <v>0.94</v>

</xml_diff>